<commit_message>
Update the result of Week 5
</commit_message>
<xml_diff>
--- a/Balance/수입및지출내역.xlsx
+++ b/Balance/수입및지출내역.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\박승빈\Desktop\IVF-SEED\Balance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC1B0765-F8D8-4D6E-9708-3852977CFAEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1A967D-40CC-473B-94AB-9F39AEC54E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18E6AD9D-570A-4E80-8DE0-36A472B1012C}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
   <si>
     <t>수입</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -151,11 +151,15 @@
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
-    <t>단체복 구매 (7인)</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
     <t>필리핀선교헌금</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>후원</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>단체복 구매 (8인)</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -676,10 +680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{018A6AAC-DC8D-46EC-87FC-9984D95AE976}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -824,7 +828,7 @@
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3"/>
       <c r="B14" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C14" s="1">
         <v>100000</v>
@@ -835,116 +839,134 @@
         <v>45747</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1">
         <v>50000</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="1">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="1">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C16">
-        <f>187+57+68+71+71+71+123+123+68</f>
-        <v>839</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="2" t="s">
+      <c r="C18">
+        <f>187+57+68+71+71+71+123+123+68+186</f>
+        <v>1025</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C19" s="1">
         <v>55</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D19" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="1">
-        <f>SUM(C3:C17)</f>
-        <v>2910894</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C19" s="1"/>
+      <c r="E19" s="1">
+        <f>SUM(C3:C19)</f>
+        <v>2951080</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="8" t="s">
+      <c r="C20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C23" s="4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C22" s="1">
-        <v>360000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B23" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23" s="1">
-        <v>360000</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="C24" s="1">
+        <v>360000</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="C25" s="1">
+        <v>360000</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B27" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D28" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="5" t="s">
+      <c r="E28" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D28" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D30" t="s">
         <v>23</v>
       </c>
-      <c r="E28" s="7">
-        <f>E17+720000</f>
-        <v>3630894</v>
-      </c>
-      <c r="F28" t="s">
+      <c r="E30" s="7">
+        <f>E19+720000</f>
+        <v>3671080</v>
+      </c>
+      <c r="F30" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -953,10 +975,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F569244-BFDB-4D19-9594-BD0DA78A671F}">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1022,78 +1044,83 @@
       <c r="C6" s="1">
         <v>-435600</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1">
-        <f>SUM(C3:C6)</f>
-        <v>-1513673</v>
-      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1">
+        <v>-213810</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1">
+        <f>SUM(C3:C7)</f>
+        <v>-1727483</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="3"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="C10" s="1"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="B11" s="10"/>
+      <c r="C11" s="11"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C12" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="2" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C11">
+      <c r="C13">
         <v>-241269</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="1">
-        <v>-210000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="D15" s="5" t="s">
+    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D17" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E15" s="6">
-        <f>SUM(C11:C15)</f>
-        <v>-451269</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.3">
-      <c r="D17" t="s">
+      <c r="E17" s="6">
+        <f>SUM(C13:C17)</f>
+        <v>-241269</v>
+      </c>
+    </row>
+    <row r="19" spans="4:5" x14ac:dyDescent="0.3">
+      <c r="D19" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="1">
-        <f>SUM(E6,E15)</f>
-        <v>-1964942</v>
+      <c r="E19" s="1">
+        <f>SUM(E7,E17)</f>
+        <v>-1968752</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A11:C11"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Itinerary for Minseok Song
</commit_message>
<xml_diff>
--- a/Balance/수입및지출내역.xlsx
+++ b/Balance/수입및지출내역.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\박승빈\Desktop\IVF-SEED\Balance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D1A967D-40CC-473B-94AB-9F39AEC54E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{499C5B69-32FD-47EF-BB27-7ACE05FDDC62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{18E6AD9D-570A-4E80-8DE0-36A472B1012C}"/>
   </bookViews>
   <sheets>
     <sheet name="수입" sheetId="1" r:id="rId1"/>
     <sheet name="지출" sheetId="2" r:id="rId2"/>
+    <sheet name="활동 중 지출 내역" sheetId="3" r:id="rId3"/>
+    <sheet name="1인 당 비용 지출" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="53">
   <si>
     <t>수입</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -160,6 +162,94 @@
   </si>
   <si>
     <t>단체복 구매 (8인)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>경주 숙소 1박 (8/9-10)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>수량</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>총액</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>식비</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>아침</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>점심</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>저녁</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>저녁-일반</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>저녁-학생</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>점심-학생</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>점심-일반</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>치킨</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>활동비</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>시장에서 음식재료 사기</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>간식</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>차량 렌트</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>한복 대여</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>동궁과 월지</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>경주월드</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>경주월드(생일할인)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>랩탑 스탠드 구매</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -231,7 +321,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -291,6 +381,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -306,7 +405,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -331,6 +430,33 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -341,6 +467,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -680,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{018A6AAC-DC8D-46EC-87FC-9984D95AE976}">
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -694,11 +823,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -864,109 +993,128 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="3">
+        <v>45751</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="1">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <f>187+57+68+71+71+71+123+123+68+186</f>
         <v>1025</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="2" t="s">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C20" s="1">
         <v>55</v>
       </c>
-      <c r="D19" s="5" t="s">
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B21" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" s="1">
+        <v>20000</v>
+      </c>
+      <c r="D21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="1">
-        <f>SUM(C3:C19)</f>
-        <v>2951080</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="C21" s="1"/>
+      <c r="E21" s="1">
+        <f>SUM(C3:C21)</f>
+        <v>3071080</v>
+      </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="8" t="s">
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="B24" s="17"/>
+      <c r="C24" s="17"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B24" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C24" s="1">
-        <v>360000</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C25" s="1">
-        <v>360000</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
+      </c>
+      <c r="C26" s="1">
+        <v>360000</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
-        <v>17</v>
+        <v>7</v>
+      </c>
+      <c r="C27" s="1">
+        <v>360000</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D30" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="5" t="s">
+      <c r="E30" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="D30" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D32" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="7">
-        <f>E19+720000</f>
-        <v>3671080</v>
-      </c>
-      <c r="F30" t="s">
+      <c r="E32" s="7">
+        <f>E21+720000</f>
+        <v>3791080</v>
+      </c>
+      <c r="F32" t="s">
         <v>24</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A24:C24"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -978,7 +1126,7 @@
   <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -989,11 +1137,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -1053,17 +1201,24 @@
       <c r="C7" s="1">
         <v>-213810</v>
       </c>
-      <c r="D7" s="5" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>45750</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="1">
+        <v>-650000</v>
+      </c>
+      <c r="D8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="1">
-        <f>SUM(C3:C7)</f>
-        <v>-1727483</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="C8" s="1"/>
+      <c r="E8" s="1">
+        <f>SUM(C3:C8)</f>
+        <v>-2377483</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
@@ -1074,11 +1229,11 @@
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="10"/>
-      <c r="C11" s="11"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="20"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
@@ -1113,8 +1268,8 @@
         <v>26</v>
       </c>
       <c r="E19" s="1">
-        <f>SUM(E7,E17)</f>
-        <v>-1968752</v>
+        <f>SUM(E8,E17)</f>
+        <v>-2618752</v>
       </c>
     </row>
   </sheetData>
@@ -1125,4 +1280,1019 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4B7EA35-A25C-4F31-87D3-1B749932A158}">
+  <dimension ref="A1:K33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="9" style="2"/>
+    <col min="5" max="5" width="10.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="G1" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
+        <v>45873</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="2">
+        <v>4500</v>
+      </c>
+      <c r="D3" s="2">
+        <v>5</v>
+      </c>
+      <c r="E3" s="8">
+        <f>C3*D3</f>
+        <v>22500</v>
+      </c>
+      <c r="G3" s="9">
+        <v>45876</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3">
+        <v>30000</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3" s="7">
+        <f t="shared" ref="K3:K6" si="0">I3*J3</f>
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2">
+        <v>5500</v>
+      </c>
+      <c r="D4" s="2">
+        <v>7</v>
+      </c>
+      <c r="E4" s="8">
+        <f t="shared" ref="E4:E31" si="1">C4*D4</f>
+        <v>38500</v>
+      </c>
+      <c r="G4" s="9">
+        <v>45877</v>
+      </c>
+      <c r="K4" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>45874</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4500</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
+      <c r="E6" s="8">
+        <f>C6*D6</f>
+        <v>22500</v>
+      </c>
+      <c r="K6" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="2">
+        <v>5500</v>
+      </c>
+      <c r="D7" s="2">
+        <v>7</v>
+      </c>
+      <c r="E7" s="8">
+        <f>C7*D7</f>
+        <v>38500</v>
+      </c>
+      <c r="G7" s="9">
+        <v>45878</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7">
+        <v>30000</v>
+      </c>
+      <c r="J7">
+        <v>12</v>
+      </c>
+      <c r="K7" s="7">
+        <f>I7*J7</f>
+        <v>360000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="2">
+        <v>10000</v>
+      </c>
+      <c r="D8" s="2">
+        <v>12</v>
+      </c>
+      <c r="E8" s="8">
+        <f t="shared" si="1"/>
+        <v>120000</v>
+      </c>
+      <c r="G8" s="9">
+        <v>45879</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8">
+        <v>3000</v>
+      </c>
+      <c r="J8">
+        <v>12</v>
+      </c>
+      <c r="K8" s="7">
+        <f>I8*J8</f>
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>45875</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E9" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="9">
+        <v>45880</v>
+      </c>
+      <c r="H9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I9">
+        <v>26000</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+      <c r="K9" s="7">
+        <f>I9*J9</f>
+        <v>26000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4500</v>
+      </c>
+      <c r="D10" s="2">
+        <v>5</v>
+      </c>
+      <c r="E10" s="8">
+        <f>C10*D10</f>
+        <v>22500</v>
+      </c>
+      <c r="H10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10">
+        <v>35400</v>
+      </c>
+      <c r="J10">
+        <v>11</v>
+      </c>
+      <c r="K10" s="7">
+        <f>I10*J10</f>
+        <v>389400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="2">
+        <v>5500</v>
+      </c>
+      <c r="D11" s="2">
+        <v>7</v>
+      </c>
+      <c r="E11" s="8">
+        <f>C11*D11</f>
+        <v>38500</v>
+      </c>
+      <c r="G11" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="7">
+        <f>SUM(K3:K10)</f>
+        <v>931400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="2">
+        <v>10000</v>
+      </c>
+      <c r="D12" s="2">
+        <v>12</v>
+      </c>
+      <c r="E12" s="8">
+        <f t="shared" si="1"/>
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>45876</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E13" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B14" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="2">
+        <v>4500</v>
+      </c>
+      <c r="D14" s="2">
+        <v>5</v>
+      </c>
+      <c r="E14" s="8">
+        <f t="shared" si="1"/>
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="2">
+        <v>5500</v>
+      </c>
+      <c r="D15" s="2">
+        <v>7</v>
+      </c>
+      <c r="E15" s="8">
+        <f t="shared" si="1"/>
+        <v>38500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>45877</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C17" s="2">
+        <v>4500</v>
+      </c>
+      <c r="D17" s="2">
+        <v>5</v>
+      </c>
+      <c r="E17" s="8">
+        <f t="shared" si="1"/>
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C18" s="2">
+        <v>5500</v>
+      </c>
+      <c r="D18" s="2">
+        <v>7</v>
+      </c>
+      <c r="E18" s="8">
+        <f t="shared" si="1"/>
+        <v>38500</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="2">
+        <v>10000</v>
+      </c>
+      <c r="D19" s="2">
+        <v>12</v>
+      </c>
+      <c r="E19" s="8">
+        <f t="shared" si="1"/>
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B20" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>45878</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E21" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="2">
+        <v>10000</v>
+      </c>
+      <c r="D22" s="2">
+        <v>12</v>
+      </c>
+      <c r="E22" s="8">
+        <f t="shared" si="1"/>
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B23" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="2">
+        <v>10000</v>
+      </c>
+      <c r="D23" s="2">
+        <v>12</v>
+      </c>
+      <c r="E23" s="8">
+        <f t="shared" si="1"/>
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="3">
+        <v>45879</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E24" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="2">
+        <v>10000</v>
+      </c>
+      <c r="D25" s="2">
+        <v>12</v>
+      </c>
+      <c r="E25" s="8">
+        <f t="shared" si="1"/>
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" s="2">
+        <v>10000</v>
+      </c>
+      <c r="D26" s="2">
+        <v>12</v>
+      </c>
+      <c r="E26" s="8">
+        <f t="shared" si="1"/>
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>45880</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E27" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="2">
+        <v>10000</v>
+      </c>
+      <c r="D28" s="2">
+        <v>12</v>
+      </c>
+      <c r="E28" s="8">
+        <f t="shared" si="1"/>
+        <v>120000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C29" s="2">
+        <v>0</v>
+      </c>
+      <c r="D29" s="2">
+        <v>0</v>
+      </c>
+      <c r="E29" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C30" s="2">
+        <v>21000</v>
+      </c>
+      <c r="D30" s="2">
+        <v>6</v>
+      </c>
+      <c r="E30" s="8">
+        <f t="shared" si="1"/>
+        <v>126000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="3">
+        <v>45881</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E31" s="8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="10">
+        <f>SUM(E3:E31)</f>
+        <v>1391000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="A33:E33"/>
+    <mergeCell ref="G11:J11"/>
+    <mergeCell ref="A32:D32"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC5FBA5-D1BA-46AB-AC14-F5516DF713B9}">
+  <dimension ref="A1:G32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" style="7"/>
+    <col min="6" max="6" width="22.5" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="E1" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>45873</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="13">
+        <v>5500</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="9">
+        <v>45876</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>45874</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="8"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="9">
+        <v>45877</v>
+      </c>
+      <c r="G4" s="7"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="8">
+        <v>5500</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="G5" s="7"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="14">
+        <v>10000</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="G6" s="7"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>45875</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="9">
+        <v>45878</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" s="7">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="8">
+        <v>5500</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="9">
+        <v>45879</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" s="7">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="13">
+        <v>10000</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="9">
+        <v>45880</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="7">
+        <v>35400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>45876</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="8"/>
+      <c r="D10" s="2"/>
+      <c r="G10" s="7"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="2"/>
+      <c r="B11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="8">
+        <v>5500</v>
+      </c>
+      <c r="D11" s="2"/>
+      <c r="E11" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="21"/>
+      <c r="G11" s="15">
+        <f>SUM(G3:G9)</f>
+        <v>68400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="13">
+        <v>10000</v>
+      </c>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>45877</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="8"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="8">
+        <v>5500</v>
+      </c>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="11"/>
+      <c r="B15" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="13">
+        <v>10000</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>45878</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="8"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="2"/>
+      <c r="B17" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="8">
+        <v>10000</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="11"/>
+      <c r="B18" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="13">
+        <v>10000</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>45879</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="8"/>
+      <c r="D19" s="2"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="2"/>
+      <c r="B20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="8">
+        <v>10000</v>
+      </c>
+      <c r="D20" s="2"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+      <c r="B21" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="13">
+        <v>10000</v>
+      </c>
+      <c r="D21" s="2"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="3">
+        <v>45880</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="8"/>
+      <c r="D22" s="2"/>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="8">
+        <v>10000</v>
+      </c>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="8">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="11"/>
+      <c r="B25" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="13">
+        <v>21000</v>
+      </c>
+      <c r="D25" s="2"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>45881</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="8"/>
+      <c r="D26" s="2"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="2"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="21"/>
+      <c r="C28" s="8">
+        <f>SUM(C3:C26)</f>
+        <v>138500</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G28" s="16">
+        <f>C28+G11</f>
+        <v>206900</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="2"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="2"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C32" s="15"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update the result of week 6
</commit_message>
<xml_diff>
--- a/Balance/수입및지출내역.xlsx
+++ b/Balance/수입및지출내역.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\박승빈\Desktop\IVF-SEED\Balance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB67A017-7E21-4B97-AB41-CE961B39BCBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C11903-605C-44E0-9230-B71E650A72F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{18E6AD9D-570A-4E80-8DE0-36A472B1012C}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="66">
   <si>
     <t>수입</t>
     <phoneticPr fontId="4" type="noConversion"/>
@@ -294,6 +294,14 @@
   </si>
   <si>
     <t>단체복 구매</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>경주 숙소 2박 (8/10-12)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>합계</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -305,7 +313,7 @@
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,8 +354,24 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="맑은 고딕"/>
+      <family val="2"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,6 +386,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -435,7 +469,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
@@ -448,8 +482,14 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -504,6 +544,9 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -513,18 +556,26 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="41" fontId="2" fillId="2" borderId="0" xfId="2" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="41" fontId="5" fillId="4" borderId="0" xfId="4" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="5" borderId="0" xfId="5" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="6">
     <cellStyle name="계산" xfId="3" builtinId="22"/>
+    <cellStyle name="나쁨" xfId="4" builtinId="27"/>
+    <cellStyle name="보통" xfId="5" builtinId="28"/>
     <cellStyle name="쉼표 [0]" xfId="1" builtinId="6"/>
     <cellStyle name="좋음" xfId="2" builtinId="26"/>
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -862,7 +913,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -880,10 +931,10 @@
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="21"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -1240,7 +1291,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1249,7 +1300,7 @@
     <col min="2" max="2" width="27.625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="2"/>
-    <col min="7" max="7" width="10" style="22" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -1258,10 +1309,10 @@
       </c>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
-      <c r="F1" s="21" t="s">
+      <c r="F1" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="21"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
@@ -1276,7 +1327,7 @@
       <c r="F2" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="G2" s="23">
+      <c r="G2" s="1">
         <f>SUM(C3:C6,C9:C10)</f>
         <v>-1882184</v>
       </c>
@@ -1294,9 +1345,9 @@
       <c r="F3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="G3" s="23">
-        <f>C8</f>
-        <v>-650000</v>
+      <c r="G3" s="1">
+        <f>C8+C11</f>
+        <v>-1150480</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -1309,7 +1360,7 @@
       <c r="F4" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="G4" s="23">
+      <c r="G4" s="1">
         <f>SUM(C7)</f>
         <v>-213810</v>
       </c>
@@ -1336,9 +1387,9 @@
       <c r="F6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="23">
+      <c r="G6" s="1">
         <f>SUM(G2:G4)</f>
-        <v>-2745994</v>
+        <v>-3246474</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -1360,6 +1411,13 @@
       <c r="C8" s="1">
         <v>-650000</v>
       </c>
+      <c r="F8" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="22">
+        <f>수입!E33</f>
+        <v>4491080</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
@@ -1370,6 +1428,13 @@
       </c>
       <c r="C9" s="1">
         <v>-260800</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" s="24">
+        <f>E12</f>
+        <v>-3246474</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1380,30 +1445,46 @@
       <c r="C10" s="1">
         <v>-107711</v>
       </c>
+      <c r="F10" s="25" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="26">
+        <f>SUM(G8:G9)</f>
+        <v>1244606</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="D11" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E11" s="1">
-        <f>SUM(C3:C10)</f>
-        <v>-2745994</v>
+      <c r="A11" s="3">
+        <v>45756</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C11" s="1">
+        <v>-500480</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
       <c r="C12" s="1"/>
+      <c r="D12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="1">
+        <f>SUM(C3:C12)</f>
+        <v>-3246474</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="20"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="21"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
@@ -1438,8 +1519,8 @@
         <v>25</v>
       </c>
       <c r="E22" s="1">
-        <f>SUM(E11,E20)</f>
-        <v>-2987263</v>
+        <f>SUM(E12,E20)</f>
+        <v>-3487743</v>
       </c>
     </row>
   </sheetData>
@@ -1458,7 +1539,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O19" sqref="O19"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1471,20 +1552,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="G1" s="21" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="G1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -1744,12 +1825,12 @@
         <f>C11*D11</f>
         <v>38500</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="21"/>
-      <c r="I11" s="21"/>
-      <c r="J11" s="21"/>
+      <c r="H11" s="18"/>
+      <c r="I11" s="18"/>
+      <c r="J11" s="18"/>
       <c r="K11" s="7">
         <f>SUM(K3:K10)</f>
         <v>931400</v>
@@ -2037,25 +2118,25 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B32" s="21"/>
-      <c r="C32" s="21"/>
-      <c r="D32" s="21"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
       <c r="E32" s="10">
         <f>SUM(E3:E31)</f>
         <v>1391000</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="21" t="s">
+      <c r="A33" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="B33" s="21"/>
-      <c r="C33" s="21"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="21"/>
+      <c r="B33" s="18"/>
+      <c r="C33" s="18"/>
+      <c r="D33" s="18"/>
+      <c r="E33" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2075,7 +2156,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2087,16 +2168,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="E1" s="21" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="E1" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="12" t="s">
@@ -2252,10 +2333,10 @@
         <v>5500</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="21"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="15">
         <f>SUM(G3:G9)</f>
         <v>68400</v>
@@ -2418,10 +2499,10 @@
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="21" t="s">
+      <c r="A28" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B28" s="21"/>
+      <c r="B28" s="18"/>
       <c r="C28" s="8">
         <f>SUM(C3:C26)</f>
         <v>138500</v>

</xml_diff>